<commit_message>
created mile stione report and images
</commit_message>
<xml_diff>
--- a/timelog.xlsx
+++ b/timelog.xlsx
@@ -24,18 +24,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>pileup parser</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Task</t>
   </si>
   <si>
-    <t>Time Hours</t>
+    <t>SVG Creator</t>
   </si>
   <si>
-    <t>SVG Creator</t>
+    <t>Flow Diagram</t>
+  </si>
+  <si>
+    <t>Pileup Parser</t>
+  </si>
+  <si>
+    <t>Hours Spent</t>
   </si>
 </sst>
 </file>
@@ -353,10 +356,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D3:E5"/>
+  <dimension ref="D3:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D3" sqref="D3:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -366,25 +369,33 @@
   <sheetData>
     <row r="3" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D4" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5">
         <v>3</v>
       </c>
-      <c r="E5">
+    </row>
+    <row r="6" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6">
         <v>2</v>
       </c>
     </row>

</xml_diff>